<commit_message>
finished test data validation by pandas.
</commit_message>
<xml_diff>
--- a/DM/test.xlsx
+++ b/DM/test.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
-  <si>
-    <t>KEY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -57,6 +54,27 @@
   </si>
   <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>XXX_KEY</t>
+  </si>
+  <si>
+    <t>TEST_VALUE</t>
+  </si>
+  <si>
+    <t>ADDRESS_KEY</t>
+  </si>
+  <si>
+    <t>STORE_KEY</t>
+  </si>
+  <si>
+    <t>NULL_ID</t>
+  </si>
+  <si>
+    <t>NULL_NM</t>
+  </si>
+  <si>
+    <t>M_KEY</t>
   </si>
 </sst>
 </file>
@@ -394,32 +412,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K2" sqref="K2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,16 +463,25 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>43523</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+      <c r="K2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -444,13 +489,22 @@
         <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
         <v>43524</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="K3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -458,13 +512,22 @@
         <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <v>43525</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -472,13 +535,22 @@
         <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>43526</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -486,16 +558,25 @@
         <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
         <v>43527</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -503,13 +584,22 @@
         <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
         <v>43528</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -517,13 +607,22 @@
         <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>43529</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -531,13 +630,22 @@
         <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <v>43530</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -545,10 +653,19 @@
         <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
         <v>43531</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>